<commit_message>
updated time in research log
</commit_message>
<xml_diff>
--- a/Research.Work Log.xlsx
+++ b/Research.Work Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cp159\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spring 2020\PikaHunt\CS4900-Game-Design-master\CS4900-Game-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75C98B01-5DE3-4A0C-9F9F-F9C9EC07FC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE35DA29-A5D8-4A64-A78F-6FAA8AEFD4CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D1B427D6-EE17-451A-8480-6D07DC71A08B}"/>
+    <workbookView xWindow="5850" yWindow="3165" windowWidth="12180" windowHeight="7260" xr2:uid="{D1B427D6-EE17-451A-8480-6D07DC71A08B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>Subject</t>
+  </si>
+  <si>
+    <t>Haley</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>Researching how to use blender, working on textures</t>
   </si>
 </sst>
 </file>
@@ -393,20 +402,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F8A96F-CA46-41E3-A53D-536DA30BC5B4}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,6 +424,17 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>